<commit_message>
just copied the data structure
</commit_message>
<xml_diff>
--- a/data/av_estimates.xlsx
+++ b/data/av_estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e72fa63d99f79ef2/Documents/Uni Agrarwissenschaften/Master/10. Semester/Decision Analysis/DecisionAnalysis_Agrivoltaics2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C62965D-6360-4D3C-9B9B-3FF5306C4E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{9C62965D-6360-4D3C-9B9B-3FF5306C4E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3B5F692-31AC-40B0-B82C-DEA4B16B3D84}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C20753DB-C6E2-4303-8131-94BE362EE1B2}"/>
+    <workbookView xWindow="30270" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{C20753DB-C6E2-4303-8131-94BE362EE1B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -433,11 +433,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F58BC73-43D5-48C5-9CB3-CCAEF2C96FD7}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>